<commit_message>
Update Test Results 2024052802_Baseline.xlsx
</commit_message>
<xml_diff>
--- a/BoxerTest/test output/Test Results 2024052802_Baseline.xlsx
+++ b/BoxerTest/test output/Test Results 2024052802_Baseline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fac223c63165d4aa/Braid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Braid Technologies\BraidTechnologiesRepo\WorkedExamples\BoxerTest\test output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F729B2B-6BE1-4D50-9509-9E79FB64A3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E463066-D408-4C31-B21C-91D36C549353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{627C950B-E8BE-43A1-969F-9B558CB032C1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{627C950B-E8BE-43A1-969F-9B558CB032C1}"/>
   </bookViews>
   <sheets>
     <sheet name="test_output" sheetId="2" r:id="rId1"/>
@@ -656,13 +656,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0169E17B-0B00-4B1F-BFEC-8D4A4E16F284}" name="test_output" displayName="test_output" ref="A1:F100" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F100" xr:uid="{0169E17B-0B00-4B1F-BFEC-8D4A4E16F284}">
-    <filterColumn colId="3">
-      <customFilters>
-        <customFilter operator="lessThan" val="0.8"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F100">
     <sortCondition descending="1" ref="D1:D100"/>
   </sortState>
@@ -1001,16 +994,16 @@
       <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="55.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +1023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1050,7 +1043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1070,7 +1063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1090,7 +1083,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -1110,7 +1103,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1130,7 +1123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1150,7 +1143,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -1170,7 +1163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -1190,7 +1183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1210,7 +1203,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1230,7 +1223,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1250,7 +1243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -1270,7 +1263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -1290,7 +1283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -1310,7 +1303,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -1330,7 +1323,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -1350,7 +1343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -1370,7 +1363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>169</v>
       </c>
@@ -1390,7 +1383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -1410,7 +1403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -1430,7 +1423,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1450,7 +1443,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>168</v>
       </c>
@@ -1470,7 +1463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1490,7 +1483,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -1510,7 +1503,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -1530,7 +1523,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -1550,7 +1543,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1570,7 +1563,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -1590,7 +1583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -1610,7 +1603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>137</v>
       </c>
@@ -1630,7 +1623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1650,7 +1643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1670,7 +1663,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -1690,7 +1683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>149</v>
       </c>
@@ -1710,7 +1703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>135</v>
       </c>
@@ -1730,7 +1723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -1750,7 +1743,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -1770,7 +1763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -1790,7 +1783,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>171</v>
       </c>
@@ -1810,7 +1803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1830,7 +1823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>94</v>
       </c>
@@ -1850,7 +1843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>122</v>
       </c>
@@ -1870,7 +1863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -1890,7 +1883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>108</v>
       </c>
@@ -1910,7 +1903,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -1930,7 +1923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>98</v>
       </c>
@@ -1950,7 +1943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>152</v>
       </c>
@@ -1970,7 +1963,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -1990,7 +1983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>127</v>
       </c>
@@ -2010,7 +2003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>153</v>
       </c>
@@ -2030,7 +2023,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -2050,7 +2043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>142</v>
       </c>
@@ -2070,7 +2063,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -2090,7 +2083,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>148</v>
       </c>
@@ -2110,7 +2103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>113</v>
       </c>
@@ -2130,7 +2123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -2150,7 +2143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>106</v>
       </c>
@@ -2170,7 +2163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>87</v>
       </c>
@@ -2190,7 +2183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>159</v>
       </c>
@@ -2210,7 +2203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>96</v>
       </c>
@@ -2230,7 +2223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>88</v>
       </c>
@@ -2250,7 +2243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>97</v>
       </c>
@@ -2270,7 +2263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>174</v>
       </c>
@@ -2290,7 +2283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>140</v>
       </c>
@@ -2310,7 +2303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>162</v>
       </c>
@@ -2330,7 +2323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>156</v>
       </c>
@@ -2350,7 +2343,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>42</v>
       </c>
@@ -2370,7 +2363,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>112</v>
       </c>
@@ -2390,7 +2383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>144</v>
       </c>
@@ -2410,7 +2403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>114</v>
       </c>
@@ -2430,7 +2423,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>165</v>
       </c>
@@ -2450,7 +2443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>123</v>
       </c>
@@ -2470,7 +2463,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -2490,7 +2483,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>141</v>
       </c>
@@ -2510,7 +2503,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>173</v>
       </c>
@@ -2530,7 +2523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>164</v>
       </c>
@@ -2550,7 +2543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>151</v>
       </c>
@@ -2570,7 +2563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>145</v>
       </c>
@@ -2590,7 +2583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>177</v>
       </c>
@@ -2610,7 +2603,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>46</v>
       </c>
@@ -2630,7 +2623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>170</v>
       </c>
@@ -2650,7 +2643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>29</v>
       </c>
@@ -2670,7 +2663,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>104</v>
       </c>
@@ -2690,7 +2683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>163</v>
       </c>
@@ -2710,7 +2703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>105</v>
       </c>
@@ -2730,7 +2723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>91</v>
       </c>
@@ -2750,7 +2743,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>45</v>
       </c>
@@ -2770,7 +2763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>172</v>
       </c>
@@ -2790,7 +2783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -2810,7 +2803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>150</v>
       </c>
@@ -2830,7 +2823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>117</v>
       </c>
@@ -2850,7 +2843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>134</v>
       </c>
@@ -2870,7 +2863,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>56</v>
       </c>
@@ -2890,7 +2883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>120</v>
       </c>
@@ -2910,7 +2903,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>99</v>
       </c>
@@ -2930,7 +2923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>32</v>
       </c>
@@ -2950,7 +2943,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>100</v>
       </c>
@@ -2970,7 +2963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>136</v>
       </c>
@@ -2990,7 +2983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>57</v>
       </c>
@@ -3024,7 +3017,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>